<commit_message>
cell type mapping and preliminary correlation
</commit_message>
<xml_diff>
--- a/tables/cell_type_mapping.xlsx
+++ b/tables/cell_type_mapping.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
-    <sheet name="cell_type_mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="extended mapping" sheetId="2" r:id="rId2"/>
+    <sheet name="mapping_to_gold_standard" sheetId="3" r:id="rId1"/>
+    <sheet name="cell_type_mapping" sheetId="1" r:id="rId2"/>
+    <sheet name="extended mapping" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
   <si>
     <t>IKDC</t>
   </si>
@@ -217,6 +218,45 @@
   </si>
   <si>
     <t>T reg</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>CD4+ T cells</t>
+  </si>
+  <si>
+    <t>CD8+ T cells</t>
+  </si>
+  <si>
+    <t>regulatory T cells</t>
+  </si>
+  <si>
+    <t>B cells</t>
+  </si>
+  <si>
+    <t>Macrophages/Monocytes</t>
+  </si>
+  <si>
+    <t>Dendritic cells</t>
+  </si>
+  <si>
+    <t>Natural killer cells</t>
+  </si>
+  <si>
+    <t>Cancer associated fibroblasts</t>
+  </si>
+  <si>
+    <t>Ovarian carcinoma cells</t>
+  </si>
+  <si>
+    <t>Melanoma cells</t>
+  </si>
+  <si>
+    <t>gold standard</t>
+  </si>
+  <si>
+    <t>gold_standard</t>
   </si>
 </sst>
 </file>
@@ -276,7 +316,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -292,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -588,13 +628,420 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
@@ -1059,7 +1506,7 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1110,21 +1557,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +1705,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1266,7 +1717,9 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1276,7 +1729,9 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>

</xml_diff>